<commit_message>
Update for key to Shaoyong Zhang
</commit_message>
<xml_diff>
--- a/信北A315钥匙记录表-谭琳.xlsx
+++ b/信北A315钥匙记录表-谭琳.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhenghaiyong/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhenghaiyong/workspace/GitHub/zhenglab/stuff/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -111,9 +111,6 @@
     <t>崔金娜</t>
   </si>
   <si>
-    <t>陶虹</t>
-  </si>
-  <si>
     <t>谭琳</t>
   </si>
   <si>
@@ -151,6 +148,13 @@
       </rPr>
       <t>钥匙拥有情况</t>
     </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>张少永</t>
+    <rPh sb="0" eb="1">
+      <t>zhang shao yong</t>
+    </rPh>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -503,7 +507,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -639,7 +643,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Withdraw the key from FanJiaojiao
</commit_message>
<xml_diff>
--- a/信北A315钥匙记录表-谭琳.xlsx
+++ b/信北A315钥匙记录表-谭琳.xlsx
@@ -27,14 +27,80 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>郑海永</t>
+  </si>
+  <si>
+    <t>俞智斌</t>
+  </si>
+  <si>
+    <t>常琳</t>
+  </si>
+  <si>
+    <t>王焱</t>
+  </si>
+  <si>
+    <t>张齐齐</t>
+  </si>
+  <si>
+    <t>孙凤娜</t>
+  </si>
+  <si>
+    <t>汤宁</t>
+  </si>
+  <si>
+    <t>王超</t>
+  </si>
+  <si>
+    <t>崔金娜</t>
+  </si>
+  <si>
+    <t>谭琳</t>
+  </si>
+  <si>
+    <t>丁昊</t>
+  </si>
+  <si>
+    <t>李娜</t>
+  </si>
+  <si>
+    <t>姜善宸</t>
+  </si>
+  <si>
+    <t>郑自强</t>
+  </si>
+  <si>
+    <r>
+      <t>信北A</t>
+    </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>315</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
       </rPr>
+      <t>钥匙拥有情况</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>张少永</t>
+    <rPh sb="0" eb="1">
+      <t>zhang shao yong</t>
+    </rPh>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t>（目前共</t>
     </r>
     <r>
@@ -57,7 +123,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>16</t>
+      <t>15</t>
     </r>
     <r>
       <rPr>
@@ -65,96 +131,8 @@
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>把，闲置</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t>把）</t>
-    </r>
-  </si>
-  <si>
-    <t>郑海永</t>
-  </si>
-  <si>
-    <t>俞智斌</t>
-  </si>
-  <si>
-    <t>常琳</t>
-  </si>
-  <si>
-    <t>王焱</t>
-  </si>
-  <si>
-    <t>张齐齐</t>
-  </si>
-  <si>
-    <t>孙凤娜</t>
-  </si>
-  <si>
-    <t>汤宁</t>
-  </si>
-  <si>
-    <t>王超</t>
-  </si>
-  <si>
-    <t>崔金娜</t>
-  </si>
-  <si>
-    <t>谭琳</t>
-  </si>
-  <si>
-    <t>丁昊</t>
-  </si>
-  <si>
-    <t>李娜</t>
-  </si>
-  <si>
-    <t>姜善宸</t>
-  </si>
-  <si>
-    <t>郑自强</t>
-  </si>
-  <si>
-    <t>范娇娇</t>
-  </si>
-  <si>
-    <r>
-      <t>信北A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>315</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t>钥匙拥有情况</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>张少永</t>
-    <rPh sb="0" eb="1">
-      <t>zhang shao yong</t>
-    </rPh>
+      <t>把，闲置4把）</t>
+    </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -494,7 +472,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -507,13 +485,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -523,7 +501,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -531,7 +509,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -539,7 +517,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
@@ -547,7 +525,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
@@ -555,7 +533,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
@@ -563,7 +541,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
@@ -571,7 +549,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
@@ -579,7 +557,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
@@ -587,7 +565,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
@@ -595,7 +573,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
@@ -603,7 +581,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
@@ -611,7 +589,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
@@ -619,7 +597,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
@@ -627,7 +605,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
@@ -635,28 +613,25 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Withdraw the keys from SunFengna, WangYan, and ZhangQiqi
</commit_message>
<xml_diff>
--- a/信北A315钥匙记录表-谭琳.xlsx
+++ b/信北A315钥匙记录表-谭琳.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>郑海永</t>
   </si>
@@ -36,15 +36,6 @@
   </si>
   <si>
     <t>常琳</t>
-  </si>
-  <si>
-    <t>王焱</t>
-  </si>
-  <si>
-    <t>张齐齐</t>
-  </si>
-  <si>
-    <t>孙凤娜</t>
   </si>
   <si>
     <t>汤宁</t>
@@ -123,7 +114,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>15</t>
+      <t>12</t>
     </r>
     <r>
       <rPr>
@@ -131,7 +122,7 @@
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>把，闲置4把）</t>
+      <t>把，闲置7把）</t>
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -472,7 +463,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -485,13 +476,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -589,30 +580,21 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Grant the keys to LuJingyu and DuAngang
</commit_message>
<xml_diff>
--- a/信北A315钥匙记录表-谭琳.xlsx
+++ b/信北A315钥匙记录表-谭琳.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>郑海永</t>
   </si>
@@ -91,6 +91,23 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>卢婧宇</t>
+    <rPh sb="0" eb="1">
+      <t>lu jing yu</t>
+    </rPh>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>杜昂昂</t>
+    <rPh sb="0" eb="1">
+      <t>du ang</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ang</t>
+    </rPh>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t>（目前共</t>
     </r>
@@ -114,7 +131,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>12</t>
+      <t>14</t>
     </r>
     <r>
       <rPr>
@@ -122,7 +139,7 @@
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>把，闲置7把）</t>
+      <t>把，闲置5把）</t>
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -463,7 +480,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -482,7 +499,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -587,9 +604,15 @@
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Withdraw the key from ChangLin
</commit_message>
<xml_diff>
--- a/信北A315钥匙记录表-谭琳.xlsx
+++ b/信北A315钥匙记录表-谭琳.xlsx
@@ -27,15 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>郑海永</t>
   </si>
   <si>
     <t>俞智斌</t>
-  </si>
-  <si>
-    <t>常琳</t>
   </si>
   <si>
     <t>汤宁</t>
@@ -131,7 +128,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>14</t>
+      <t>13</t>
     </r>
     <r>
       <rPr>
@@ -139,7 +136,7 @@
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>把，闲置5把）</t>
+      <t>把，闲置6把）</t>
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -480,7 +477,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -493,13 +490,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -589,7 +586,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
@@ -610,9 +607,6 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Withdraw the key from TanLin and update server info file
</commit_message>
<xml_diff>
--- a/信北A315钥匙记录表-谭琳.xlsx
+++ b/信北A315钥匙记录表-谭琳.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10880" yWindow="820" windowWidth="24240" windowHeight="12740" tabRatio="990"/>
+    <workbookView xWindow="1360" yWindow="820" windowWidth="24240" windowHeight="12740" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>郑海永</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>崔金娜</t>
-  </si>
-  <si>
-    <t>谭琳</t>
   </si>
   <si>
     <t>丁昊</t>
@@ -128,7 +125,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>13</t>
+      <t>12</t>
     </r>
     <r>
       <rPr>
@@ -136,7 +133,7 @@
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>把，闲置6把）</t>
+      <t>把，闲置7把）</t>
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -490,13 +487,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -578,7 +575,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
@@ -599,9 +596,6 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Withdraw the key from DingHao
</commit_message>
<xml_diff>
--- a/信北A315钥匙记录表-谭琳.xlsx
+++ b/信北A315钥匙记录表-谭琳.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>郑海永</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>崔金娜</t>
-  </si>
-  <si>
-    <t>丁昊</t>
   </si>
   <si>
     <t>李娜</t>
@@ -125,7 +122,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>12</t>
+      <t>11</t>
     </r>
     <r>
       <rPr>
@@ -133,7 +130,7 @@
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>把，闲置7把）</t>
+      <t>把，闲置8把）</t>
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -487,13 +484,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -567,7 +564,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
@@ -588,9 +585,6 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Grant the keys to GuoZemin, QiuChenchen, ZhangHaoxu, LiuJing, and ZhaoYan
</commit_message>
<xml_diff>
--- a/信北A315钥匙记录表-谭琳.xlsx
+++ b/信北A315钥匙记录表-谭琳.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>郑海永</t>
   </si>
@@ -99,6 +99,34 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>郭泽民</t>
+    <rPh sb="0" eb="1">
+      <t>guo ze m</t>
+    </rPh>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>邱晨晨</t>
+    <rPh sb="0" eb="1">
+      <t>qiu chen c</t>
+    </rPh>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>刘静</t>
+    <rPh sb="0" eb="1">
+      <t>liu jing</t>
+    </rPh>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>赵燕</t>
+    <rPh sb="0" eb="1">
+      <t>zhao yan</t>
+    </rPh>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t>（目前共</t>
     </r>
@@ -122,7 +150,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>11</t>
+      <t>16</t>
     </r>
     <r>
       <rPr>
@@ -130,8 +158,18 @@
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>把，闲置8把）</t>
-    </r>
+      <t>把，闲置3把）</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>张皓旭</t>
+    <rPh sb="0" eb="1">
+      <t>zhang</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>hao</t>
+    </rPh>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -471,7 +509,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="E1" sqref="E1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -490,7 +528,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -587,38 +625,53 @@
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Grant the key to YuanHao
</commit_message>
<xml_diff>
--- a/信北A315钥匙记录表-谭琳.xlsx
+++ b/信北A315钥匙记录表-谭琳.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>郑海永</t>
   </si>
@@ -123,6 +123,23 @@
     <t>赵燕</t>
     <rPh sb="0" eb="1">
       <t>zhao yan</t>
+    </rPh>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>张皓旭</t>
+    <rPh sb="0" eb="1">
+      <t>zhang</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>hao</t>
+    </rPh>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>苑浩</t>
+    <rPh sb="0" eb="1">
+      <t>yuan hao</t>
     </rPh>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -150,7 +167,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>16</t>
+      <t>17</t>
     </r>
     <r>
       <rPr>
@@ -158,18 +175,8 @@
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>把，闲置3把）</t>
+      <t>把，闲置2把）</t>
     </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>张皓旭</t>
-    <rPh sb="0" eb="1">
-      <t>zhang</t>
-    </rPh>
-    <rPh sb="1" eb="2">
-      <t>hao</t>
-    </rPh>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -528,7 +535,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -642,7 +649,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
@@ -663,6 +670,9 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Grant the key to LinGuoting
</commit_message>
<xml_diff>
--- a/信北A315钥匙记录表-谭琳.xlsx
+++ b/信北A315钥匙记录表-谭琳.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>郑海永</t>
   </si>
@@ -167,7 +167,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>17</t>
+      <t>18</t>
     </r>
     <r>
       <rPr>
@@ -175,8 +175,21 @@
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>把，闲置2把）</t>
+      <t>把，闲置1把）</t>
     </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>林国婷</t>
+    <rPh sb="0" eb="1">
+      <t>lin guo ting</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>guo</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ting</t>
+    </rPh>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -680,6 +693,9 @@
       <c r="A19">
         <v>18</v>
       </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20">

</xml_diff>